<commit_message>
Add Transport and Cities Management
</commit_message>
<xml_diff>
--- a/download/model.xlsx
+++ b/download/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\Excel\src\main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\order_mission\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>ESITH/DAF</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Petit Déjeuner</t>
-  </si>
-  <si>
-    <t>VP ZAIM</t>
   </si>
   <si>
     <t>Déjeuner et Diner</t>
@@ -217,8 +214,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-40C]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -564,53 +562,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -930,7 +928,7 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E34" sqref="E34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -949,10 +947,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="59"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="K1" s="2"/>
@@ -994,10 +992,10 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="47"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1018,16 +1016,16 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
       <c r="G10" s="2"/>
       <c r="H10" s="4">
         <v>2015</v>
@@ -1050,10 +1048,10 @@
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="47"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1130,15 +1128,15 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="49" t="s">
+      <c r="B16" s="56"/>
+      <c r="C16" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
       <c r="F16" s="3" t="s">
         <v>19</v>
       </c>
@@ -1168,10 +1166,10 @@
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="9">
         <v>80</v>
       </c>
@@ -1206,10 +1204,10 @@
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="9">
         <v>280</v>
       </c>
@@ -1244,13 +1242,13 @@
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="62"/>
       <c r="F22" s="13" t="s">
         <v>27</v>
       </c>
@@ -1261,10 +1259,10 @@
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="51"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="14" t="s">
         <v>29</v>
       </c>
@@ -1303,10 +1301,10 @@
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="54"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="21">
         <v>1</v>
       </c>
@@ -1318,13 +1316,23 @@
         <f>SUM(C25*D25)</f>
         <v>20.25</v>
       </c>
-      <c r="F25" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="22"/>
-      <c r="H25" s="12"/>
+      <c r="F25" s="22" t="str">
+        <f>C16</f>
+        <v>Voiture personnelle</v>
+      </c>
+      <c r="G25" s="22">
+        <f>H16</f>
+        <v>738</v>
+      </c>
+      <c r="H25" s="12">
+        <f>H20</f>
+        <v>1.8</v>
+      </c>
       <c r="I25" s="23"/>
-      <c r="J25" s="22"/>
+      <c r="J25" s="22">
+        <f>SUM(G25*H25)</f>
+        <v>1328.4</v>
+      </c>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1339,10 +1347,10 @@
       <c r="K26" s="26"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="54"/>
+      <c r="A27" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="50"/>
       <c r="C27" s="21">
         <v>2</v>
       </c>
@@ -1358,7 +1366,10 @@
       <c r="G27" s="22"/>
       <c r="H27" s="27"/>
       <c r="I27" s="23"/>
-      <c r="J27" s="22"/>
+      <c r="J27" s="22">
+        <f>SUM(G27*H27)</f>
+        <v>0</v>
+      </c>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
@@ -1400,10 +1411,10 @@
       <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="54"/>
+      <c r="A31" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="50"/>
       <c r="C31" s="21">
         <v>1</v>
       </c>
@@ -1436,39 +1447,39 @@
     </row>
     <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
-      <c r="B33" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
+      <c r="B33" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
       <c r="E33" s="36">
         <f>SUM(E24:E32)</f>
         <v>460.25</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G33" s="38"/>
       <c r="H33" s="38"/>
       <c r="I33" s="39"/>
       <c r="J33" s="40">
         <f>SUM(J24:J32)</f>
-        <v>0</v>
+        <v>1328.4</v>
       </c>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="62">
+      <c r="B34" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="63">
         <f>SUM(E33+J33)</f>
-        <v>460.25</v>
-      </c>
-      <c r="F34" s="63"/>
+        <v>1788.65</v>
+      </c>
+      <c r="F34" s="64"/>
       <c r="G34" s="41"/>
       <c r="H34" s="41"/>
       <c r="I34" s="11"/>
@@ -1502,12 +1513,12 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
+      <c r="A37" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
       <c r="G37" s="42"/>
       <c r="H37" s="2"/>
       <c r="K37" s="43"/>
@@ -1517,7 +1528,7 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E38" s="41"/>
       <c r="F38" s="41"/>
@@ -1543,13 +1554,13 @@
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="42" t="s">
         <v>43</v>
-      </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="42" t="s">
-        <v>44</v>
       </c>
       <c r="E40" s="42"/>
       <c r="F40" s="42"/>
@@ -1573,11 +1584,11 @@
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
+      <c r="A42" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
       <c r="D42" s="42">
         <v>2016</v>
       </c>
@@ -1597,7 +1608,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H43" s="44"/>
       <c r="I43" s="2"/>
@@ -1611,7 +1622,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -1645,11 +1656,11 @@
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="59"/>
-      <c r="C47" s="59"/>
+      <c r="A47" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -1659,11 +1670,11 @@
       <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="59"/>
-      <c r="C48" s="59"/>
+      <c r="A48" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -1709,95 +1720,120 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
+      <c r="D52" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D53" s="64" t="s">
+      <c r="D53" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D54" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D54" s="64" t="s">
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G58" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="64"/>
-      <c r="F54" s="64"/>
-    </row>
-    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G58" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="H58" s="55"/>
+      <c r="H58" s="53"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G59" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H59" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="H59" s="45" t="s">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G60" s="54"/>
+      <c r="H60" s="54"/>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="46"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="55"/>
+    </row>
+    <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="46" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
-    </row>
-    <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="B61" s="58"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="57"/>
-    </row>
-    <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="58" t="s">
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A63" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="58"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="58"/>
-      <c r="K62" s="1"/>
-    </row>
-    <row r="63" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="58" t="s">
+      <c r="B63" s="46"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="K63" s="1"/>
-    </row>
-    <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="58" t="s">
+      <c r="B64" s="46"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="46"/>
+    </row>
+    <row r="65" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A65" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
-    </row>
-    <row r="65" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A65" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" s="58"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
+      <c r="B65" s="46"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="46"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="K65" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G60:H61"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="A62:D62"/>
     <mergeCell ref="A63:D63"/>
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="A65:D65"/>
@@ -1805,31 +1841,6 @@
     <mergeCell ref="D52:F52"/>
     <mergeCell ref="D53:F53"/>
     <mergeCell ref="D54:F54"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G60:H61"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="C16:E16"/>
   </mergeCells>
   <pageMargins left="0.37" right="0.17" top="0.57999999999999996" bottom="0.28999999999999998" header="0.51181102362204722" footer="0.28999999999999998"/>
   <pageSetup paperSize="9" scale="57" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Search by Criteria and entreprise Management
</commit_message>
<xml_diff>
--- a/download/model.xlsx
+++ b/download/model.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>ESITH/DAF</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Monsieur, Mme, Melle :</t>
   </si>
   <si>
-    <t xml:space="preserve">EL FATIHI MOHAMED </t>
-  </si>
-  <si>
     <t>TOTAL (2)</t>
   </si>
   <si>
@@ -62,30 +59,18 @@
     <t>Destination :</t>
   </si>
   <si>
-    <t>TANGER</t>
-  </si>
-  <si>
     <t>Date départ :</t>
   </si>
   <si>
     <t>Heures :</t>
   </si>
   <si>
-    <t>22H00</t>
-  </si>
-  <si>
     <t>Date retour :</t>
   </si>
   <si>
-    <t>20H00</t>
-  </si>
-  <si>
     <t>Moyen de Transport utilisé :</t>
   </si>
   <si>
-    <t>Voiture personnelle</t>
-  </si>
-  <si>
     <t>Distance Trajet ( A/R ) :</t>
   </si>
   <si>
@@ -152,13 +137,7 @@
     <t>Arrété le présent décompte à la somme de :</t>
   </si>
   <si>
-    <t>QUATRE CENT SOIXANTE DIRHAMS.</t>
-  </si>
-  <si>
     <t>Imputation Budgétaire :</t>
-  </si>
-  <si>
-    <t>Mission au maroc</t>
   </si>
   <si>
     <t>Exercice Budgétaire :</t>
@@ -562,53 +541,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -927,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -947,10 +926,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="46"/>
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="K1" s="2"/>
@@ -992,10 +971,10 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="47"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1016,20 +995,16 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="4">
-        <v>2015</v>
-      </c>
+      <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1048,25 +1023,23 @@
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1087,31 +1060,23 @@
     </row>
     <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="6">
-        <v>42551</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="6">
-        <v>42552</v>
-      </c>
+      <c r="G14" s="6"/>
       <c r="H14" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="J14" s="9"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
@@ -1128,27 +1093,25 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
+      <c r="A16" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="58"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
       <c r="F16" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="9">
-        <v>738</v>
+        <v>0</v>
       </c>
       <c r="I16" s="9">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K16" s="10"/>
     </row>
@@ -1166,27 +1129,27 @@
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="47"/>
+      <c r="A18" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="58"/>
       <c r="C18" s="9">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="9">
-        <v>20.25</v>
+        <v>0</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K18" s="12"/>
     </row>
@@ -1204,27 +1167,27 @@
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="47"/>
+      <c r="A20" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="58"/>
       <c r="C20" s="9">
-        <v>280</v>
+        <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="9">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K20" s="12"/>
     </row>
@@ -1242,15 +1205,15 @@
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
+      <c r="A22" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="64"/>
       <c r="F22" s="13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
@@ -1259,31 +1222,31 @@
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="60"/>
+      <c r="C23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>33</v>
-      </c>
       <c r="H23" s="15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I23" s="16"/>
       <c r="J23" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K23" s="12"/>
     </row>
@@ -1301,37 +1264,37 @@
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="54"/>
+      <c r="A25" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="50"/>
       <c r="C25" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="22">
         <f>H18</f>
-        <v>20.25</v>
+        <v>0</v>
       </c>
       <c r="E25" s="22">
         <f>SUM(C25*D25)</f>
-        <v>20.25</v>
-      </c>
-      <c r="F25" s="22" t="str">
+        <v>0</v>
+      </c>
+      <c r="F25" s="22">
         <f>C16</f>
-        <v>Voiture personnelle</v>
+        <v>0</v>
       </c>
       <c r="G25" s="22">
-        <f>H16</f>
-        <v>738</v>
+        <f>H16+I16</f>
+        <v>0</v>
       </c>
       <c r="H25" s="12">
         <f>H20</f>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="22">
         <f>SUM(G25*H25)</f>
-        <v>1328.4</v>
+        <v>0</v>
       </c>
       <c r="K25" s="12"/>
     </row>
@@ -1347,20 +1310,20 @@
       <c r="K26" s="26"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="54"/>
+      <c r="A27" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="50"/>
       <c r="C27" s="21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27" s="22">
         <f>C18</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E27" s="22">
         <f>SUM(C27*D27)</f>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
@@ -1411,20 +1374,20 @@
       <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="54"/>
+      <c r="A31" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="50"/>
       <c r="C31" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="22">
         <f>SUM(C20)</f>
-        <v>280</v>
+        <v>0</v>
       </c>
       <c r="E31" s="22">
         <f>SUM(C31*D31)</f>
-        <v>280</v>
+        <v>0</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="29"/>
@@ -1447,39 +1410,39 @@
     </row>
     <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
-      <c r="B33" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
+      <c r="B33" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
       <c r="E33" s="36">
         <f>SUM(E24:E32)</f>
-        <v>460.25</v>
+        <v>0</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G33" s="38"/>
       <c r="H33" s="38"/>
       <c r="I33" s="39"/>
       <c r="J33" s="40">
         <f>SUM(J24:J32)</f>
-        <v>1328.4</v>
+        <v>0</v>
       </c>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="62">
+      <c r="B34" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="53">
         <f>SUM(E33+J33)</f>
-        <v>1788.65</v>
-      </c>
-      <c r="F34" s="63"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="41"/>
       <c r="H34" s="41"/>
       <c r="I34" s="11"/>
@@ -1513,12 +1476,12 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
+      <c r="A37" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
       <c r="G37" s="42"/>
       <c r="H37" s="2"/>
       <c r="K37" s="43"/>
@@ -1527,14 +1490,12 @@
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="D38" s="41"/>
       <c r="E38" s="41"/>
       <c r="F38" s="41"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I38" s="41"/>
       <c r="J38" s="3"/>
@@ -1554,14 +1515,12 @@
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="42" t="s">
-        <v>43</v>
-      </c>
+      <c r="A40" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="58"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="42"/>
       <c r="E40" s="42"/>
       <c r="F40" s="42"/>
       <c r="G40" s="5"/>
@@ -1584,14 +1543,12 @@
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="42">
-        <v>2016</v>
-      </c>
+      <c r="A42" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="42"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -1608,7 +1565,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="44" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H43" s="44"/>
       <c r="I43" s="2"/>
@@ -1622,7 +1579,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -1656,11 +1613,11 @@
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="59"/>
-      <c r="C47" s="59"/>
+      <c r="A47" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -1670,11 +1627,11 @@
       <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="59"/>
-      <c r="C48" s="59"/>
+      <c r="A48" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -1701,7 +1658,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -1720,40 +1677,40 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
+      <c r="D52" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D53" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
+      <c r="D53" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D54" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="E54" s="64"/>
-      <c r="F54" s="64"/>
+      <c r="D54" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G58" s="55" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H58" s="55"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G59" s="45" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -1761,54 +1718,79 @@
       <c r="H60" s="56"/>
     </row>
     <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="B61" s="58"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
+      <c r="A61" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="46"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
       <c r="G61" s="56"/>
       <c r="H61" s="57"/>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B62" s="58"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="58"/>
+      <c r="A62" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
       <c r="K62" s="1"/>
     </row>
     <row r="63" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
+      <c r="A63" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" s="46"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
       <c r="K63" s="1"/>
     </row>
     <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
+      <c r="A64" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B64" s="46"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="46"/>
     </row>
     <row r="65" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A65" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="B65" s="58"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
+      <c r="A65" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" s="46"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="46"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="K65" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G60:H61"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="A62:D62"/>
     <mergeCell ref="A63:D63"/>
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="A65:D65"/>
@@ -1816,31 +1798,6 @@
     <mergeCell ref="D52:F52"/>
     <mergeCell ref="D53:F53"/>
     <mergeCell ref="D54:F54"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G60:H61"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="C16:E16"/>
   </mergeCells>
   <pageMargins left="0.37" right="0.17" top="0.57999999999999996" bottom="0.28999999999999998" header="0.51181102362204722" footer="0.28999999999999998"/>
   <pageSetup paperSize="9" scale="57" orientation="portrait" r:id="rId1"/>

</xml_diff>